<commit_message>
admin panel updated, added function which is adding food from admin panel.
</commit_message>
<xml_diff>
--- a/src/main/resources/royxat.xlsx
+++ b/src/main/resources/royxat.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Ism Familya</t>
   </si>
@@ -26,40 +26,19 @@
     <t>Vaqt</t>
   </si>
   <si>
-    <t>Sherbek</t>
+    <t>Fazliddin Xamdamov</t>
   </si>
   <si>
-    <t>Asistent</t>
+    <t>Assistant</t>
   </si>
   <si>
     <t>Osh</t>
   </si>
   <si>
-    <t>2022-03-12T08:01:24</t>
+    <t>2022-03-14T12:49:23.242951</t>
   </si>
   <si>
-    <t>Bekjon</t>
-  </si>
-  <si>
-    <t>HR</t>
-  </si>
-  <si>
-    <t>Chauchvara</t>
-  </si>
-  <si>
-    <t>2022-03-12T08:01:28</t>
-  </si>
-  <si>
-    <t>Faazliddin</t>
-  </si>
-  <si>
-    <t>Mentor</t>
-  </si>
-  <si>
-    <t>Bedri</t>
-  </si>
-  <si>
-    <t>2022-03-12T08:01:27</t>
+    <t>2022-03-14T13:22:13.154746</t>
   </si>
 </sst>
 </file>
@@ -104,7 +83,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -140,30 +119,16 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>